<commit_message>
- added + and - markings on in and out - improved ground traces
</commit_message>
<xml_diff>
--- a/TPS63031 breakout.xlsx
+++ b/TPS63031 breakout.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
-  <si>
-    <t>Part</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Value</t>
   </si>
@@ -140,6 +137,12 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>š+</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1042,191 +1045,196 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>